<commit_message>
Finished first part of clustering sota
</commit_message>
<xml_diff>
--- a/slr/clustering.xlsx
+++ b/slr/clustering.xlsx
@@ -1094,7 +1094,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="50.8515625"/>
     <col customWidth="1" min="5" max="5" width="17.00390625"/>
@@ -1556,194 +1556,194 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
+    <row r="10" s="1" customFormat="1">
+      <c r="A10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>2018</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>72</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>83</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>90</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>476</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s">
+    <row r="11" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>2017</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>17</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>26</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>426</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
+    <row r="12" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>2018</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>465</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>20</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>417</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
+    <row r="13" s="2" customFormat="1">
+      <c r="A13" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>2014</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>46</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>198</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <v>226</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="2">
         <v>411</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="2" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1894,50 +1894,50 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="17" s="1" customFormat="1">
+      <c r="A17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>2015</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>1855</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>1870</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="1">
         <v>363</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2132,50 +2132,50 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="22" s="1" customFormat="1">
+      <c r="A22" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>2016</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>99</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>135</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
         <v>145</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>306</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="1" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>